<commit_message>
Complete refactoring of old SmartFurniture code structure and various bug-fixes
</commit_message>
<xml_diff>
--- a/output/bucatarie_trifan_input_output/Comanda_Proficut_Alex Trifan.xlsx
+++ b/output/bucatarie_trifan_input_output/Comanda_Proficut_Alex Trifan.xlsx
@@ -1670,7 +1670,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="106" t="n"/>
-      <c r="K10" s="107" t="n"/>
+      <c r="K10" s="107" t="inlineStr"/>
       <c r="W10" s="49">
         <f>A10*B10*C10/1000000</f>
         <v/>
@@ -1767,7 +1767,7 @@
       <c r="H11" s="108" t="inlineStr"/>
       <c r="I11" s="109" t="inlineStr"/>
       <c r="J11" s="106" t="n"/>
-      <c r="K11" s="110" t="n"/>
+      <c r="K11" s="110" t="inlineStr"/>
       <c r="M11" s="48" t="n"/>
       <c r="W11" s="49">
         <f>A11*B11*C11/1000000</f>
@@ -1865,7 +1865,7 @@
       <c r="H12" s="108" t="inlineStr"/>
       <c r="I12" s="109" t="inlineStr"/>
       <c r="J12" s="106" t="n"/>
-      <c r="K12" s="110" t="n"/>
+      <c r="K12" s="110" t="inlineStr"/>
       <c r="W12" s="49">
         <f>A12*B12*C12/1000000</f>
         <v/>
@@ -1964,7 +1964,7 @@
       <c r="H13" s="108" t="inlineStr"/>
       <c r="I13" s="109" t="inlineStr"/>
       <c r="J13" s="106" t="n"/>
-      <c r="K13" s="110" t="n"/>
+      <c r="K13" s="110" t="inlineStr"/>
       <c r="M13" s="66" t="n"/>
       <c r="W13" s="49">
         <f>A13*B13*C13/1000000</f>
@@ -2064,7 +2064,7 @@
       <c r="H14" s="108" t="inlineStr"/>
       <c r="I14" s="109" t="inlineStr"/>
       <c r="J14" s="106" t="n"/>
-      <c r="K14" s="110" t="n"/>
+      <c r="K14" s="110" t="inlineStr"/>
       <c r="M14" s="66" t="n"/>
       <c r="W14" s="49">
         <f>A14*B14*C14/1000000</f>
@@ -2162,7 +2162,7 @@
       <c r="H15" s="108" t="inlineStr"/>
       <c r="I15" s="109" t="inlineStr"/>
       <c r="J15" s="106" t="n"/>
-      <c r="K15" s="110" t="n"/>
+      <c r="K15" s="110" t="inlineStr"/>
       <c r="M15" s="66" t="n"/>
       <c r="W15" s="49">
         <f>A15*B15*C15/1000000</f>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="106" t="n"/>
-      <c r="K16" s="110" t="n"/>
+      <c r="K16" s="110" t="inlineStr"/>
       <c r="M16" s="66" t="n"/>
       <c r="W16" s="49">
         <f>A16*B16*C16/1000000</f>
@@ -2362,7 +2362,7 @@
       <c r="H17" s="108" t="inlineStr"/>
       <c r="I17" s="109" t="inlineStr"/>
       <c r="J17" s="106" t="n"/>
-      <c r="K17" s="110" t="n"/>
+      <c r="K17" s="110" t="inlineStr"/>
       <c r="M17" s="66" t="n"/>
       <c r="W17" s="49">
         <f>A17*B17*C17/1000000</f>
@@ -2460,7 +2460,7 @@
       <c r="H18" s="108" t="inlineStr"/>
       <c r="I18" s="109" t="inlineStr"/>
       <c r="J18" s="106" t="n"/>
-      <c r="K18" s="110" t="n"/>
+      <c r="K18" s="110" t="inlineStr"/>
       <c r="M18" s="66" t="n"/>
       <c r="W18" s="49">
         <f>A18*B18*C18/1000000</f>
@@ -2558,7 +2558,7 @@
       <c r="H19" s="108" t="inlineStr"/>
       <c r="I19" s="109" t="inlineStr"/>
       <c r="J19" s="106" t="n"/>
-      <c r="K19" s="110" t="n"/>
+      <c r="K19" s="110" t="inlineStr"/>
       <c r="M19" s="66" t="n"/>
       <c r="W19" s="49">
         <f>A19*B19*C19/1000000</f>
@@ -2656,7 +2656,7 @@
       <c r="H20" s="108" t="inlineStr"/>
       <c r="I20" s="109" t="inlineStr"/>
       <c r="J20" s="106" t="n"/>
-      <c r="K20" s="110" t="n"/>
+      <c r="K20" s="110" t="inlineStr"/>
       <c r="M20" s="48" t="n"/>
       <c r="W20" s="49">
         <f>A20*B20*C20/1000000</f>
@@ -2754,7 +2754,7 @@
       <c r="H21" s="108" t="inlineStr"/>
       <c r="I21" s="109" t="inlineStr"/>
       <c r="J21" s="109" t="n"/>
-      <c r="K21" s="110" t="n"/>
+      <c r="K21" s="110" t="inlineStr"/>
       <c r="M21" s="48" t="n"/>
       <c r="W21" s="49">
         <f>A21*B21*C21/1000000</f>
@@ -2852,7 +2852,7 @@
       <c r="H22" s="108" t="inlineStr"/>
       <c r="I22" s="109" t="inlineStr"/>
       <c r="J22" s="109" t="n"/>
-      <c r="K22" s="110" t="n"/>
+      <c r="K22" s="110" t="inlineStr"/>
       <c r="M22" s="48" t="n"/>
       <c r="W22" s="49">
         <f>A22*B22*C22/1000000</f>
@@ -2950,7 +2950,7 @@
       <c r="H23" s="108" t="inlineStr"/>
       <c r="I23" s="109" t="inlineStr"/>
       <c r="J23" s="109" t="n"/>
-      <c r="K23" s="110" t="n"/>
+      <c r="K23" s="110" t="inlineStr"/>
       <c r="M23" s="66" t="n"/>
       <c r="W23" s="49">
         <f>A23*B23*C23/1000000</f>
@@ -3048,7 +3048,7 @@
       <c r="H24" s="108" t="inlineStr"/>
       <c r="I24" s="109" t="inlineStr"/>
       <c r="J24" s="109" t="n"/>
-      <c r="K24" s="110" t="n"/>
+      <c r="K24" s="110" t="inlineStr"/>
       <c r="W24" s="49">
         <f>A24*B24*C24/1000000</f>
         <v/>
@@ -3145,7 +3145,7 @@
       <c r="H25" s="108" t="inlineStr"/>
       <c r="I25" s="109" t="inlineStr"/>
       <c r="J25" s="109" t="n"/>
-      <c r="K25" s="110" t="n"/>
+      <c r="K25" s="110" t="inlineStr"/>
       <c r="W25" s="49">
         <f>A25*B25*C25/1000000</f>
         <v/>
@@ -3242,7 +3242,7 @@
       <c r="H26" s="108" t="inlineStr"/>
       <c r="I26" s="109" t="inlineStr"/>
       <c r="J26" s="109" t="n"/>
-      <c r="K26" s="110" t="n"/>
+      <c r="K26" s="110" t="inlineStr"/>
       <c r="W26" s="49">
         <f>A26*B26*C26/1000000</f>
         <v/>

</xml_diff>